<commit_message>
add sheet 2 on fetch data
</commit_message>
<xml_diff>
--- a/internal/api/files/recap_submissions.xlsx
+++ b/internal/api/files/recap_submissions.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -47,6 +48,57 @@
   </si>
   <si>
     <t xml:space="preserve">Unlock Answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toxin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood</t>
   </si>
 </sst>
 </file>
@@ -230,10 +282,10 @@
   <dimension ref="A2:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
@@ -284,4 +336,105 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:S2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="16.94"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>